<commit_message>
Update lesson 29 DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_092022\SeleniumTestNG092022Parallel\src\test\resources\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ED43D1-46EB-40EE-98DD-B242412FA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C69225-0C18-431E-9CD3-9382C84F7FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="23010" windowHeight="13725" xr2:uid="{1C8BC18A-1893-44DC-824E-B01686B47E0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1C8BC18A-1893-44DC-824E-B01686B47E0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>EMAIL</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>admin123@example.com</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
   <si>
     <t>Passed</t>
@@ -109,12 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -436,7 +440,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -462,19 +466,22 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>123456</v>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>123456</v>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lesson 30 take screenshot and record video
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>EMAIL</t>
   </si>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -119,6 +119,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -469,7 +475,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update lesson 31 Test Listener in TestNG
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>EMAIL</t>
   </si>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -119,6 +119,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -475,7 +478,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update lesson 32 Log4j2
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>EMAIL</t>
   </si>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -119,6 +119,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -478,7 +481,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update lesson 33 - Extent Report
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>EMAIL</t>
   </si>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -119,6 +119,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -481,7 +493,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update lesson 34 - Allure Report
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_092022\SeleniumTestNG092022Parallel\src\test\resources\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C69225-0C18-431E-9CD3-9382C84F7FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B32C0DB-4CE7-4582-AF6F-9410E98F7053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1C8BC18A-1893-44DC-824E-B01686B47E0C}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="23040" windowHeight="12120" xr2:uid="{1C8BC18A-1893-44DC-824E-B01686B47E0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>EMAIL</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>admin@example.com</t>
-  </si>
-  <si>
-    <t>admin123@example.com</t>
   </si>
   <si>
     <t/>
@@ -55,8 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +79,21 @@
       <color theme="10"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -95,7 +106,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
@@ -111,42 +122,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,18 +452,18 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="29.6640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="13.77734375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="9.44140625"/>
-    <col min="4" max="16384" style="1" width="8.88671875"/>
+    <col min="1" max="1" width="29.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,26 +474,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Selenium 4.9.1 and Headless mode
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_092022\SeleniumTestNG092022Parallel\src\test\resources\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B32C0DB-4CE7-4582-AF6F-9410E98F7053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D5BE04-C431-4482-9A00-D9E859BD8A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="23040" windowHeight="12120" xr2:uid="{1C8BC18A-1893-44DC-824E-B01686B47E0C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1C8BC18A-1893-44DC-824E-B01686B47E0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>EMAIL</t>
   </si>
@@ -131,11 +131,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -459,7 +459,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -493,13 +493,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Selenium 4.15.0 support CDP 119
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>EMAIL</t>
   </si>
@@ -126,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -136,6 +136,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -497,7 +503,7 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Selenium Java 4.19.1
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest/CRM.xlsx
+++ b/src/test/resources/datatest/CRM.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>EMAIL</t>
   </si>
@@ -126,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -136,6 +136,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
@@ -503,7 +506,7 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>